<commit_message>
login fallido con bloqueo tras 3 intentos
</commit_message>
<xml_diff>
--- a/src/test/resources/datos/LoginData.xlsx
+++ b/src/test/resources/datos/LoginData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{4E61E797-B8F4-47E4-89DA-BFB340DFBC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3DFEC647-A7E3-4EE1-8967-0C3B319D5EAF}"/>
+    <workbookView xWindow="23664" yWindow="624" windowWidth="17280" windowHeight="8880" xr2:uid="{3DFEC647-A7E3-4EE1-8967-0C3B319D5EAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>